<commit_message>
updated to run continously
</commit_message>
<xml_diff>
--- a/google.xlsx
+++ b/google.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -435,15 +435,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>05.30.2019, 23:30:44</t>
+          <t>06.02.2019, 22:42:39</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">

</xml_diff>